<commit_message>
inicio de visualizacion de paises
</commit_message>
<xml_diff>
--- a/analisis/resultados/argentina/costos.xlsx
+++ b/analisis/resultados/argentina/costos.xlsx
@@ -1105,7 +1105,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1209,11 +1209,11 @@
         <v>1997</v>
       </c>
       <c r="B49">
-        <v>4.348309897898337</v>
+        <v>10.02154264552858</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1227,11 +1227,11 @@
         <v>1998</v>
       </c>
       <c r="B50">
-        <v>3.431066541980492</v>
+        <v>6.564068037090995</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1245,11 +1245,11 @@
         <v>1999</v>
       </c>
       <c r="B51">
-        <v>4.034535653859936</v>
+        <v>9.156910604924347</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1263,11 +1263,11 @@
         <v>2000</v>
       </c>
       <c r="B52">
-        <v>5.413123846421029</v>
+        <v>14.03924140416419</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1281,11 +1281,11 @@
         <v>2001</v>
       </c>
       <c r="B53">
-        <v>4.846855476143246</v>
+        <v>11.18015821598729</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1299,11 +1299,11 @@
         <v>2002</v>
       </c>
       <c r="B54">
-        <v>3.62525463419652</v>
+        <v>6.039871827719271</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1317,11 +1317,11 @@
         <v>2003</v>
       </c>
       <c r="B55">
-        <v>4.201352414167802</v>
+        <v>7.466465050297496</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1335,11 +1335,11 @@
         <v>2004</v>
       </c>
       <c r="B56">
-        <v>7.221188577022128</v>
+        <v>7.636867481217681</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1353,11 +1353,11 @@
         <v>2005</v>
       </c>
       <c r="B57">
-        <v>9.026230138053835</v>
+        <v>8.803083440442739</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1371,11 +1371,11 @@
         <v>2006</v>
       </c>
       <c r="B58">
-        <v>10.56330267805366</v>
+        <v>11.65414131088522</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1389,11 +1389,11 @@
         <v>2007</v>
       </c>
       <c r="B59">
-        <v>13.9306960897557</v>
+        <v>14.09724983579705</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1407,11 +1407,11 @@
         <v>2008</v>
       </c>
       <c r="B60">
-        <v>16.75890931442544</v>
+        <v>16.87092470750025</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1425,11 +1425,11 @@
         <v>2009</v>
       </c>
       <c r="B61">
-        <v>14.90040555548995</v>
+        <v>14.82161676785997</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1443,11 +1443,11 @@
         <v>2010</v>
       </c>
       <c r="B62">
-        <v>17.54517746949896</v>
+        <v>17.62837777096416</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1461,11 +1461,11 @@
         <v>2011</v>
       </c>
       <c r="B63">
-        <v>19.79698550582703</v>
+        <v>23.0656320320991</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1479,11 +1479,11 @@
         <v>2012</v>
       </c>
       <c r="B64">
-        <v>27.31559743634367</v>
+        <v>26.38578606501133</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1497,11 +1497,11 @@
         <v>2013</v>
       </c>
       <c r="B65">
-        <v>15.99170382766293</v>
+        <v>29.58253788187292</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1515,11 +1515,11 @@
         <v>2014</v>
       </c>
       <c r="B66">
-        <v>16.58130809877055</v>
+        <v>25.59702003976075</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1533,11 +1533,11 @@
         <v>2015</v>
       </c>
       <c r="B67">
-        <v>14.04842373144222</v>
+        <v>24.26300522059164</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1551,11 +1551,11 @@
         <v>2016</v>
       </c>
       <c r="B68">
-        <v>13.64838197989061</v>
+        <v>21.97031226820259</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1569,11 +1569,11 @@
         <v>2017</v>
       </c>
       <c r="B69">
-        <v>13.65723482346044</v>
+        <v>23.10442440072572</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1587,11 +1587,11 @@
         <v>2018</v>
       </c>
       <c r="B70">
-        <v>14.41025138862266</v>
+        <v>17.54025290647301</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Propia (CCNN)</t>
+          <t>Propia (Empalme CCNN)</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">

</xml_diff>